<commit_message>
Split of File Access Screen file into two files. One for accessing the files and another to grade
</commit_message>
<xml_diff>
--- a/ExportedCSVFiles/CS4125-1.xlsx
+++ b/ExportedCSVFiles/CS4125-1.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catha\PycharmProjects\Inspector_Application\ExportedCSVFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0792DC15-2E04-4FD6-885B-C20A248B700D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-28898" yWindow="-5497" windowWidth="28996" windowHeight="16395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="15">
   <si>
     <t>aid</t>
   </si>
@@ -64,11 +70,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mmm d yyyy hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="mmm\ d\ yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +112,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -152,7 +166,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -184,9 +198,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -218,6 +250,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -393,18 +443,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,7 +486,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -459,10 +512,10 @@
         <v>11</v>
       </c>
       <c r="I2" s="1">
-        <v>43931.7500378632</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>43931.750037863203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -488,10 +541,10 @@
         <v>11</v>
       </c>
       <c r="I3" s="1">
-        <v>43931.75036031856</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>43931.750360318561</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -517,12 +570,12 @@
         <v>11</v>
       </c>
       <c r="I4" s="1">
-        <v>43932.88789175529</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>43932.887891755287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -534,22 +587,22 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>12345678</v>
+        <v>16208102</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G5">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="H5" t="s">
         <v>11</v>
       </c>
       <c r="I5" s="1">
-        <v>43932.89717781235</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>43936.750031970783</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9</v>
       </c>
@@ -575,10 +628,10 @@
         <v>11</v>
       </c>
       <c r="I6" s="1">
-        <v>43932.89964816512</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>43932.899648165119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
@@ -604,10 +657,10 @@
         <v>11</v>
       </c>
       <c r="I7" s="1">
-        <v>43932.89971429636</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>43932.899714296364</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>11</v>
       </c>
@@ -633,10 +686,10 @@
         <v>11</v>
       </c>
       <c r="I8" s="1">
-        <v>43932.89977640036</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>43932.899776400358</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>12</v>
       </c>
@@ -662,10 +715,10 @@
         <v>11</v>
       </c>
       <c r="I9" s="1">
-        <v>43932.89984315536</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>43932.899843155363</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>13</v>
       </c>
@@ -694,7 +747,7 @@
         <v>43932.89990955095</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>14</v>
       </c>
@@ -720,10 +773,10 @@
         <v>11</v>
       </c>
       <c r="I11" s="1">
-        <v>43932.89999330155</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>43932.899993301551</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -749,12 +802,12 @@
         <v>11</v>
       </c>
       <c r="I12" s="1">
-        <v>43932.8972388817</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>43932.897238881698</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -766,10 +819,10 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>16208102</v>
+        <v>111111111</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G13">
         <v>70</v>
@@ -778,7 +831,36 @@
         <v>11</v>
       </c>
       <c r="I13" s="1">
-        <v>43932.88803153412</v>
+        <v>43937.96865753649</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>12345678</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <v>25</v>
+      </c>
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="1">
+        <v>43932.897177812352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented email system to allow for multiple attachments to be sent to a student
</commit_message>
<xml_diff>
--- a/ExportedCSVFiles/CS4125-1.xlsx
+++ b/ExportedCSVFiles/CS4125-1.xlsx
@@ -446,7 +446,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -458,19 +458,19 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>111111111</v>
+        <v>161234234</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="1">
-        <v>43939.64802196829</v>
+        <v>43939.6482203932</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
@@ -478,7 +478,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -490,19 +490,19 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>12345678</v>
+        <v>16153444</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
       </c>
       <c r="G3">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="H3" t="s">
         <v>12</v>
       </c>
       <c r="I3" s="1">
-        <v>43939.64813562379</v>
+        <v>43939.6483930324</v>
       </c>
       <c r="J3" t="s">
         <v>13</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -522,19 +522,19 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>161234234</v>
+        <v>16153548</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G4">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="1">
-        <v>43939.6482203932</v>
+        <v>43939.64850693</v>
       </c>
       <c r="J4" t="s">
         <v>13</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -554,19 +554,19 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>16153444</v>
+        <v>16153724</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
       </c>
       <c r="G5">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="H5" t="s">
         <v>12</v>
       </c>
       <c r="I5" s="1">
-        <v>43939.6483930324</v>
+        <v>43939.64858319313</v>
       </c>
       <c r="J5" t="s">
         <v>13</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -586,19 +586,19 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>16153548</v>
+        <v>16153732</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
       </c>
       <c r="G6">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="H6" t="s">
         <v>12</v>
       </c>
       <c r="I6" s="1">
-        <v>43939.64850693</v>
+        <v>43939.64871062421</v>
       </c>
       <c r="J6" t="s">
         <v>13</v>
@@ -606,7 +606,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -618,19 +618,19 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>16153724</v>
+        <v>16153774</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
       </c>
       <c r="G7">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="H7" t="s">
         <v>12</v>
       </c>
       <c r="I7" s="1">
-        <v>43939.64858319313</v>
+        <v>43939.64880775208</v>
       </c>
       <c r="J7" t="s">
         <v>13</v>
@@ -638,7 +638,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -650,19 +650,19 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>16153732</v>
+        <v>16153778</v>
       </c>
       <c r="F8" t="s">
         <v>14</v>
       </c>
       <c r="G8">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="H8" t="s">
         <v>12</v>
       </c>
       <c r="I8" s="1">
-        <v>43939.64871062421</v>
+        <v>43939.6488825323</v>
       </c>
       <c r="J8" t="s">
         <v>13</v>
@@ -670,7 +670,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -682,19 +682,19 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>16153774</v>
+        <v>16161616</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G9">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="H9" t="s">
         <v>12</v>
       </c>
       <c r="I9" s="1">
-        <v>43939.64880775208</v>
+        <v>43939.64895240435</v>
       </c>
       <c r="J9" t="s">
         <v>13</v>
@@ -702,7 +702,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -714,19 +714,19 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>16153778</v>
+        <v>16161818</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G10">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="H10" t="s">
         <v>12</v>
       </c>
       <c r="I10" s="1">
-        <v>43939.6488825323</v>
+        <v>43939.64902314368</v>
       </c>
       <c r="J10" t="s">
         <v>13</v>
@@ -734,7 +734,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -746,19 +746,19 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>16161616</v>
+        <v>16208102</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G11">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="H11" t="s">
         <v>12</v>
       </c>
       <c r="I11" s="1">
-        <v>43939.64895240435</v>
+        <v>43939.64911034461</v>
       </c>
       <c r="J11" t="s">
         <v>13</v>
@@ -766,7 +766,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -778,10 +778,10 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>16161818</v>
+        <v>1622222</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G12">
         <v>25</v>
@@ -790,7 +790,7 @@
         <v>12</v>
       </c>
       <c r="I12" s="1">
-        <v>43939.64902314368</v>
+        <v>43939.64917522902</v>
       </c>
       <c r="J12" t="s">
         <v>13</v>
@@ -798,7 +798,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -810,19 +810,19 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>16208102</v>
+        <v>78945614</v>
       </c>
       <c r="F13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G13">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="H13" t="s">
         <v>12</v>
       </c>
       <c r="I13" s="1">
-        <v>43939.64911034461</v>
+        <v>43939.64928587439</v>
       </c>
       <c r="J13" t="s">
         <v>13</v>
@@ -830,7 +830,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -842,19 +842,19 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>1622222</v>
+        <v>111111111</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G14">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="H14" t="s">
         <v>12</v>
       </c>
       <c r="I14" s="1">
-        <v>43939.64917522902</v>
+        <v>43939.64802196829</v>
       </c>
       <c r="J14" t="s">
         <v>13</v>
@@ -862,7 +862,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -874,19 +874,19 @@
         <v>1</v>
       </c>
       <c r="E15">
-        <v>78945614</v>
+        <v>12345678</v>
       </c>
       <c r="F15" t="s">
         <v>14</v>
       </c>
       <c r="G15">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="H15" t="s">
         <v>12</v>
       </c>
       <c r="I15" s="1">
-        <v>43939.64928587439</v>
+        <v>43939.64813562379</v>
       </c>
       <c r="J15" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Added categories for grading
</commit_message>
<xml_diff>
--- a/ExportedCSVFiles/CS4125-1.xlsx
+++ b/ExportedCSVFiles/CS4125-1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="20">
   <si>
     <t>aid</t>
   </si>
@@ -65,6 +65,15 @@
   </si>
   <si>
     <t>test1.txt</t>
+  </si>
+  <si>
+    <t>C:\Users\catha\OneDrive - University of Limerick\Assignments3</t>
+  </si>
+  <si>
+    <t>analytics.java</t>
+  </si>
+  <si>
+    <t>C:\Users\catha\OneDrive\Desktop\OneDrive\Assignments2</t>
   </si>
 </sst>
 </file>
@@ -400,7 +409,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -830,7 +839,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -842,7 +851,7 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>111111111</v>
+        <v>16100001</v>
       </c>
       <c r="F14" t="s">
         <v>11</v>
@@ -854,41 +863,105 @@
         <v>12</v>
       </c>
       <c r="I14" s="1">
-        <v>43939.64802196829</v>
+        <v>43942.66351386514</v>
       </c>
       <c r="J14" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>16208102</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15">
+        <v>40</v>
+      </c>
+      <c r="H15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="1">
+        <v>43941.50085259893</v>
+      </c>
+      <c r="J15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16">
         <v>3</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
         <v>12345678</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F16" t="s">
         <v>14</v>
       </c>
-      <c r="G15">
-        <v>25</v>
-      </c>
-      <c r="H15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I15" s="1">
+      <c r="G16">
+        <v>40</v>
+      </c>
+      <c r="H16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="1">
         <v>43939.64813562379</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>111111111</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17">
+        <v>55</v>
+      </c>
+      <c r="H17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="1">
+        <v>43939.64802196829</v>
+      </c>
+      <c r="J17" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented multiple files in students assignments for user analytics screen
</commit_message>
<xml_diff>
--- a/ExportedCSVFiles/CS4125-1.xlsx
+++ b/ExportedCSVFiles/CS4125-1.xlsx
@@ -1,26 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catha\PycharmProjects\Inspector_Application\ExportedCSVFiles\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A400AE9-7433-48E3-A4C4-C6A5064A891A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3488" yWindow="1913" windowWidth="21600" windowHeight="11872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$200</definedName>
+  </definedNames>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="13">
   <si>
     <t>modulecode</t>
   </si>
@@ -46,38 +43,29 @@
     <t>CS4125</t>
   </si>
   <si>
+    <t>DocTest.txt</t>
+  </si>
+  <si>
+    <t>C:\Users\catha\OneDrive\Desktop\OneDrive\Assignments</t>
+  </si>
+  <si>
+    <t>DocTest - Copy (2).txt</t>
+  </si>
+  <si>
+    <t>DocTest - Copy.txt</t>
+  </si>
+  <si>
     <t>test2.txt</t>
-  </si>
-  <si>
-    <t>C:\Users\catha\OneDrive\Desktop\OneDrive\Assignments</t>
-  </si>
-  <si>
-    <t>DocTest.txt</t>
-  </si>
-  <si>
-    <t>test3.txt</t>
-  </si>
-  <si>
-    <t>test1.txt</t>
-  </si>
-  <si>
-    <t>C:\Users\catha\OneDrive - University of Limerick\Assignments3</t>
-  </si>
-  <si>
-    <t>analytics.java</t>
-  </si>
-  <si>
-    <t>C:\Users\catha\OneDrive\Desktop\OneDrive\Assignments2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mmm\ d\ yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="mmm d yyyy hh:mm:ss"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,14 +103,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -169,7 +149,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -201,27 +181,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -253,24 +215,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -446,23 +390,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.73046875" customWidth="1"/>
-    <col min="5" max="5" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.59765625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="51.73046875" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="51.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,7 +426,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -493,22 +434,22 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>161234234</v>
+        <v>16153444</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="F2" s="1">
-        <v>43939.648220393203</v>
+        <v>43945.74932839487</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -516,22 +457,22 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>16153444</v>
+        <v>16153548</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="F3" s="1">
-        <v>43939.648393032403</v>
+        <v>43945.74939740843</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -539,7 +480,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>16153548</v>
+        <v>1622222</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -548,13 +489,13 @@
         <v>25</v>
       </c>
       <c r="F4" s="1">
-        <v>43939.648506930003</v>
+        <v>43945.74851580738</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -562,45 +503,45 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>16153724</v>
+        <v>1622222</v>
       </c>
       <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>40</v>
+      </c>
+      <c r="F5" s="1">
+        <v>43945.74860676207</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1622222</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6">
         <v>10</v>
       </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1">
-        <v>43939.648583193128</v>
-      </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>16153732</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <v>100</v>
-      </c>
       <c r="F6" s="1">
-        <v>43939.648710624213</v>
+        <v>43945.74865027078</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -608,22 +549,22 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>16153774</v>
+        <v>111111111</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E7">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="F7" s="1">
-        <v>43939.648807752077</v>
+        <v>43945.74875988626</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -631,22 +572,22 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>16153778</v>
+        <v>12345678</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E8">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F8" s="1">
-        <v>43939.648882532303</v>
+        <v>43945.74884124789</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -654,22 +595,22 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>16161616</v>
+        <v>161234231</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E9">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="F9" s="1">
-        <v>43939.64895240435</v>
+        <v>43945.74891935549</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -677,22 +618,22 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>16161818</v>
+        <v>161234234</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E10">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="F10" s="1">
-        <v>43939.649023143676</v>
+        <v>43945.7489900842</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -700,22 +641,22 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>16208102</v>
+        <v>161234236</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
       <c r="E11">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="F11" s="1">
-        <v>43939.64911034461</v>
+        <v>43945.749056006</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -723,22 +664,22 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>1622222</v>
+        <v>161234237</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E12">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="F12" s="1">
-        <v>43939.649175229017</v>
+        <v>43945.74912499967</v>
       </c>
       <c r="G12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -746,229 +687,46 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>78945614</v>
+        <v>161234238</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E13">
+        <v>55</v>
+      </c>
+      <c r="F13" s="1">
+        <v>43945.74919069297</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>161234239</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14">
         <v>40</v>
       </c>
-      <c r="F13" s="1">
-        <v>43939.649285874388</v>
-      </c>
-      <c r="G13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>16100001</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14">
-        <v>55</v>
-      </c>
       <c r="F14" s="1">
-        <v>43942.66351386514</v>
+        <v>43945.74927439966</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>16208102</v>
-      </c>
-      <c r="D15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15">
-        <v>40</v>
-      </c>
-      <c r="F15" s="1">
-        <v>43941.500852598932</v>
-      </c>
-      <c r="G15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>12345678</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16">
-        <v>40</v>
-      </c>
-      <c r="F16" s="1">
-        <v>43939.648135623793</v>
-      </c>
-      <c r="G16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>111111111</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17">
-        <v>55</v>
-      </c>
-      <c r="F17" s="1">
-        <v>43939.648021968293</v>
-      </c>
-      <c r="G17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>161234231</v>
-      </c>
-      <c r="D18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18">
-        <v>85</v>
-      </c>
-      <c r="F18" s="1">
-        <v>43943.742895478783</v>
-      </c>
-      <c r="G18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>161234236</v>
-      </c>
-      <c r="D19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19">
-        <v>70</v>
-      </c>
-      <c r="F19" s="1">
-        <v>43943.743027745622</v>
-      </c>
-      <c r="G19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>161234237</v>
-      </c>
-      <c r="D20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20">
-        <v>40</v>
-      </c>
-      <c r="F20" s="1">
-        <v>43943.743121229287</v>
-      </c>
-      <c r="G20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>161234238</v>
-      </c>
-      <c r="D21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21">
-        <v>55</v>
-      </c>
-      <c r="F21" s="1">
-        <v>43943.743215176168</v>
-      </c>
-      <c r="G21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>161234239</v>
-      </c>
-      <c r="D22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22">
-        <v>25</v>
-      </c>
-      <c r="F22" s="1">
-        <v>43943.743274597247</v>
-      </c>
-      <c r="G22" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G200"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solved issue saving excel file. Now being saved where the assignments are located
</commit_message>
<xml_diff>
--- a/ExportedCSVFiles/CS4125-1.xlsx
+++ b/ExportedCSVFiles/CS4125-1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>modulecode</t>
   </si>
@@ -43,19 +43,13 @@
     <t>CS4125</t>
   </si>
   <si>
+    <t>test2.txt</t>
+  </si>
+  <si>
+    <t>C:\Users\catha\OneDrive\Desktop\OneDrive\Assignments</t>
+  </si>
+  <si>
     <t>DocTest.txt</t>
-  </si>
-  <si>
-    <t>C:\Users\catha\OneDrive\Desktop\OneDrive\Assignments</t>
-  </si>
-  <si>
-    <t>DocTest - Copy (2).txt</t>
-  </si>
-  <si>
-    <t>DocTest - Copy.txt</t>
-  </si>
-  <si>
-    <t>test2.txt</t>
   </si>
 </sst>
 </file>
@@ -391,7 +385,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -434,16 +428,16 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>16153444</v>
+        <v>111111111</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="F2" s="1">
-        <v>43945.74932839487</v>
+        <v>43947.73414990197</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -457,16 +451,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>16153548</v>
+        <v>12345678</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="F3" s="1">
-        <v>43945.74939740843</v>
+        <v>43947.73425066871</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -480,16 +474,16 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1622222</v>
+        <v>161234231</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F4" s="1">
-        <v>43945.74851580738</v>
+        <v>43947.73435902171</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
@@ -503,16 +497,16 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1622222</v>
+        <v>161234234</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E5">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F5" s="1">
-        <v>43945.74860676207</v>
+        <v>43947.73448184071</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
@@ -526,202 +520,18 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>1622222</v>
+        <v>161234236</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F6" s="1">
-        <v>43945.74865027078</v>
+        <v>43947.73462489977</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>111111111</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7">
-        <v>55</v>
-      </c>
-      <c r="F7" s="1">
-        <v>43945.74875988626</v>
-      </c>
-      <c r="G7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>12345678</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8">
-        <v>25</v>
-      </c>
-      <c r="F8" s="1">
-        <v>43945.74884124789</v>
-      </c>
-      <c r="G8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>161234231</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9">
-        <v>85</v>
-      </c>
-      <c r="F9" s="1">
-        <v>43945.74891935549</v>
-      </c>
-      <c r="G9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>161234234</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10">
-        <v>55</v>
-      </c>
-      <c r="F10" s="1">
-        <v>43945.7489900842</v>
-      </c>
-      <c r="G10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>161234236</v>
-      </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11">
-        <v>100</v>
-      </c>
-      <c r="F11" s="1">
-        <v>43945.749056006</v>
-      </c>
-      <c r="G11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>161234237</v>
-      </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12">
-        <v>55</v>
-      </c>
-      <c r="F12" s="1">
-        <v>43945.74912499967</v>
-      </c>
-      <c r="G12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>161234238</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13">
-        <v>55</v>
-      </c>
-      <c r="F13" s="1">
-        <v>43945.74919069297</v>
-      </c>
-      <c r="G13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>161234239</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14">
-        <v>40</v>
-      </c>
-      <c r="F14" s="1">
-        <v>43945.74927439966</v>
-      </c>
-      <c r="G14" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>